<commit_message>
Added Lise and Sundown mugs
Seiken Densetsu 3 and Live a Live draw near. Deciding on characters is the worst part of this.
</commit_message>
<xml_diff>
--- a/Brainstorming.xlsx
+++ b/Brainstorming.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="List of SNES RPGs" sheetId="1" r:id="rId1"/>
@@ -437,6 +437,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="F2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Because he's the main character!</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <r>
@@ -461,6 +485,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Because he's all rough and tumble?</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -482,6 +530,345 @@
           </rPr>
           <t xml:space="preserve">
 Like most DQ heroes, he lacks a true name.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The Armour of Erdrick looks armour-like, anyway.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+He's a dragon.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mains swords in a popular game, he gets to keep them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+I'd have too many clerics otherwise.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+M
+M
+M
+Magic!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Cecil is a paladin. FE paladins have horses. Git, Cecil.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+He's best known for his PSI, though I could shove him to fighter. Or cleric.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bike = horse.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bone Mail!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Because that's what summoners promote from. He can't actually cast so subject to change.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+As above, but she actually can cast and can stay in a magic class.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Flammie = pegasus.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+She uses lances, ergo soldier.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Gun = bow.</t>
         </r>
       </text>
     </comment>
@@ -490,7 +877,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="172">
   <si>
     <t>Name</t>
   </si>
@@ -991,6 +1378,21 @@
   </si>
   <si>
     <t>Note that I've finished FF1, DW1-2, and EB0, so those are fair game for me.</t>
+  </si>
+  <si>
+    <t>And now for Act 2! Not that I'll acknowledge that in game. It's too trendy.</t>
+  </si>
+  <si>
+    <t>Lise</t>
+  </si>
+  <si>
+    <t>Riesz</t>
+  </si>
+  <si>
+    <t>Soldier</t>
+  </si>
+  <si>
+    <t>Sundown</t>
   </si>
 </sst>
 </file>
@@ -1346,9 +1748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1750,9 +2150,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO18"/>
+  <dimension ref="A1:AO21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2103,14 +2503,44 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" t="s">
+        <v>169</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>171</v>
+      </c>
+      <c r="D21" t="s">
+        <v>151</v>
+      </c>
+      <c r="F21" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Properly set basic Lise/Sundown data
Faces? Check. Descriptions? Check. Forget to commit this stuff when I did it the other day? Check.
</commit_message>
<xml_diff>
--- a/Brainstorming.xlsx
+++ b/Brainstorming.xlsx
@@ -877,7 +877,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="174">
   <si>
     <t>Name</t>
   </si>
@@ -1393,6 +1393,12 @@
   </si>
   <si>
     <t>Sundown</t>
+  </si>
+  <si>
+    <t>0x10</t>
+  </si>
+  <si>
+    <t>0x11</t>
   </si>
 </sst>
 </file>
@@ -2152,7 +2158,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2528,6 +2536,9 @@
       <c r="D20" t="s">
         <v>30</v>
       </c>
+      <c r="E20" t="s">
+        <v>172</v>
+      </c>
       <c r="F20" t="s">
         <v>170</v>
       </c>
@@ -2538,6 +2549,9 @@
       </c>
       <c r="D21" t="s">
         <v>151</v>
+      </c>
+      <c r="E21" t="s">
+        <v>173</v>
       </c>
       <c r="F21" t="s">
         <v>133</v>

</xml_diff>

<commit_message>
Begun to set character stats
Now they aren't really high. They still haven't had class bases taken away, however.
</commit_message>
<xml_diff>
--- a/Brainstorming.xlsx
+++ b/Brainstorming.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr showObjects="none" filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
@@ -341,7 +341,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Don't forget to subtract class bases when inserting these.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -365,7 +389,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0" shapeId="0">
+    <comment ref="AG1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -389,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0" shapeId="0">
+    <comment ref="AL1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -877,7 +901,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="196">
   <si>
     <t>Name</t>
   </si>
@@ -1399,6 +1423,72 @@
   </si>
   <si>
     <t>0x11</t>
+  </si>
+  <si>
+    <t>Join Time</t>
+  </si>
+  <si>
+    <t>Mercenary</t>
+  </si>
+  <si>
+    <t>Cleric</t>
+  </si>
+  <si>
+    <t>Paladin</t>
+  </si>
+  <si>
+    <t>Characteristics</t>
+  </si>
+  <si>
+    <t>The main lord. Good strength, middling speed/def.</t>
+  </si>
+  <si>
+    <t>Pretty standard fighter. Big HP/strength, lowish speed, pathetic res.</t>
+  </si>
+  <si>
+    <t>Act 1's Jeigan. Str/def reasonable, forget the rest.</t>
+  </si>
+  <si>
+    <t>Do these matter? Gato, and I dunno when he'll come back. Strong enough to ruin Kaga.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He's a myrm. Big speed, not too low strength, very frail. </t>
+  </si>
+  <si>
+    <t>Look at that magic! Tempted to swap to cleric honestly. Makes more sense.</t>
+  </si>
+  <si>
+    <t>Big magic. Not much else.</t>
+  </si>
+  <si>
+    <t>A more defensive sort. Think Lowen, I suppose.</t>
+  </si>
+  <si>
+    <t>All that strength he can't use. Fairly slow.</t>
+  </si>
+  <si>
+    <t>To contrast, he can have a speed stat since the bike's old Pokemon's run.</t>
+  </si>
+  <si>
+    <t>Physical class? Strength and defence it is.</t>
+  </si>
+  <si>
+    <t>Not really sure here. Throw some skill on? Definitely change class.</t>
+  </si>
+  <si>
+    <t>Magic? Magic. Dies to a breeze? Also accurate.</t>
+  </si>
+  <si>
+    <t>Standard issue peg stats here.</t>
+  </si>
+  <si>
+    <t>Balanced in all areas.</t>
+  </si>
+  <si>
+    <t>He's a sharp shooter. Skill up.</t>
+  </si>
+  <si>
+    <t>Growth Total</t>
   </si>
 </sst>
 </file>
@@ -1468,10 +1558,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2156,10 +2247,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO21"/>
+  <dimension ref="A1:AR26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2167,7 +2258,7 @@
     <col min="4" max="4" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2187,112 +2278,121 @@
         <v>61</v>
       </c>
       <c r="G1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1" t="s">
         <v>62</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>71</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>63</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>64</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>65</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>66</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>67</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>68</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>69</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>72</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>63</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>64</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>65</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>66</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>67</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>68</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>69</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB1" t="s">
         <v>76</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>77</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>78</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>79</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>81</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>82</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>83</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>85</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>86</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>87</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>88</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>89</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>90</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>91</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -2309,10 +2409,71 @@
         <v>93</v>
       </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <v>9</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2">
+        <v>6</v>
+      </c>
+      <c r="O2">
+        <v>6</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>7</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>80</v>
+      </c>
+      <c r="T2">
+        <v>45</v>
+      </c>
+      <c r="U2">
+        <v>15</v>
+      </c>
+      <c r="V2">
+        <v>30</v>
+      </c>
+      <c r="W2">
+        <v>35</v>
+      </c>
+      <c r="X2">
+        <v>30</v>
+      </c>
+      <c r="Y2">
+        <v>10</v>
+      </c>
+      <c r="Z2">
+        <v>50</v>
+      </c>
+      <c r="AA2">
+        <f>SUM(S2:Z2)</f>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -2328,8 +2489,72 @@
       <c r="F3" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>24</v>
+      </c>
+      <c r="K3">
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>90</v>
+      </c>
+      <c r="T3">
+        <v>50</v>
+      </c>
+      <c r="U3">
+        <v>15</v>
+      </c>
+      <c r="V3">
+        <v>25</v>
+      </c>
+      <c r="W3">
+        <v>25</v>
+      </c>
+      <c r="X3">
+        <v>40</v>
+      </c>
+      <c r="Y3">
+        <v>10</v>
+      </c>
+      <c r="Z3">
+        <v>25</v>
+      </c>
+      <c r="AA3">
+        <f>SUM(S3:Z3)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -2342,8 +2567,72 @@
       <c r="F4" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>30</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>12</v>
+      </c>
+      <c r="P4">
+        <v>4</v>
+      </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>60</v>
+      </c>
+      <c r="T4">
+        <v>35</v>
+      </c>
+      <c r="U4">
+        <v>5</v>
+      </c>
+      <c r="V4">
+        <v>30</v>
+      </c>
+      <c r="W4">
+        <v>10</v>
+      </c>
+      <c r="X4">
+        <v>30</v>
+      </c>
+      <c r="Y4">
+        <v>5</v>
+      </c>
+      <c r="Z4">
+        <v>20</v>
+      </c>
+      <c r="AA4">
+        <f>SUM(S4:Z4)</f>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -2356,8 +2645,72 @@
       <c r="F5" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G5" s="2">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>45</v>
+      </c>
+      <c r="K5">
+        <v>18</v>
+      </c>
+      <c r="L5">
+        <v>12</v>
+      </c>
+      <c r="M5">
+        <v>15</v>
+      </c>
+      <c r="N5">
+        <v>15</v>
+      </c>
+      <c r="O5">
+        <v>15</v>
+      </c>
+      <c r="P5">
+        <v>12</v>
+      </c>
+      <c r="Q5">
+        <v>10</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>70</v>
+      </c>
+      <c r="T5">
+        <v>40</v>
+      </c>
+      <c r="U5">
+        <v>20</v>
+      </c>
+      <c r="V5">
+        <v>40</v>
+      </c>
+      <c r="W5">
+        <v>30</v>
+      </c>
+      <c r="X5">
+        <v>25</v>
+      </c>
+      <c r="Y5">
+        <v>10</v>
+      </c>
+      <c r="Z5">
+        <v>30</v>
+      </c>
+      <c r="AA5">
+        <f>SUM(S5:Z5)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -2370,8 +2723,72 @@
       <c r="F6" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>18</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>8</v>
+      </c>
+      <c r="N6">
+        <v>10</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>8</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>50</v>
+      </c>
+      <c r="T6">
+        <v>30</v>
+      </c>
+      <c r="U6">
+        <v>10</v>
+      </c>
+      <c r="V6">
+        <v>40</v>
+      </c>
+      <c r="W6">
+        <v>50</v>
+      </c>
+      <c r="X6">
+        <v>20</v>
+      </c>
+      <c r="Y6">
+        <v>15</v>
+      </c>
+      <c r="Z6">
+        <v>40</v>
+      </c>
+      <c r="AA6">
+        <f>SUM(S6:Z6)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -2384,8 +2801,72 @@
       <c r="F7" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>18</v>
+      </c>
+      <c r="K7" s="2">
+        <v>4</v>
+      </c>
+      <c r="L7" s="2">
+        <v>7</v>
+      </c>
+      <c r="M7" s="2">
+        <v>6</v>
+      </c>
+      <c r="N7" s="2">
+        <v>5</v>
+      </c>
+      <c r="O7" s="2">
+        <v>4</v>
+      </c>
+      <c r="P7" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>3</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2">
+        <v>45</v>
+      </c>
+      <c r="T7" s="2">
+        <v>20</v>
+      </c>
+      <c r="U7" s="2">
+        <v>40</v>
+      </c>
+      <c r="V7" s="2">
+        <v>30</v>
+      </c>
+      <c r="W7" s="2">
+        <v>25</v>
+      </c>
+      <c r="X7" s="2">
+        <v>15</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>30</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA7">
+        <f>SUM(S7:Z7)</f>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -2401,8 +2882,72 @@
       <c r="F8" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>16</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>9</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <v>5</v>
+      </c>
+      <c r="Q8">
+        <v>6</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>60</v>
+      </c>
+      <c r="T8">
+        <v>10</v>
+      </c>
+      <c r="U8">
+        <v>55</v>
+      </c>
+      <c r="V8">
+        <v>30</v>
+      </c>
+      <c r="W8">
+        <v>30</v>
+      </c>
+      <c r="X8">
+        <v>20</v>
+      </c>
+      <c r="Y8">
+        <v>30</v>
+      </c>
+      <c r="Z8">
+        <v>20</v>
+      </c>
+      <c r="AA8">
+        <f>SUM(S8:Z8)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>104</v>
       </c>
@@ -2415,8 +2960,72 @@
       <c r="F9" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>22</v>
+      </c>
+      <c r="K9">
+        <v>7</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9">
+        <v>6</v>
+      </c>
+      <c r="N9">
+        <v>4</v>
+      </c>
+      <c r="O9">
+        <v>8</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="Q9">
+        <v>8</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>90</v>
+      </c>
+      <c r="T9">
+        <v>30</v>
+      </c>
+      <c r="U9">
+        <v>10</v>
+      </c>
+      <c r="V9">
+        <v>40</v>
+      </c>
+      <c r="W9">
+        <v>25</v>
+      </c>
+      <c r="X9">
+        <v>40</v>
+      </c>
+      <c r="Y9">
+        <v>10</v>
+      </c>
+      <c r="Z9">
+        <v>40</v>
+      </c>
+      <c r="AA9">
+        <f>SUM(S9:Z9)</f>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -2429,8 +3038,72 @@
       <c r="F10" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G10" s="2">
+        <v>2</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>24</v>
+      </c>
+      <c r="K10" s="2">
+        <v>6</v>
+      </c>
+      <c r="L10" s="2">
+        <v>4</v>
+      </c>
+      <c r="M10" s="2">
+        <v>5</v>
+      </c>
+      <c r="N10" s="2">
+        <v>5</v>
+      </c>
+      <c r="O10" s="2">
+        <v>5</v>
+      </c>
+      <c r="P10" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>7</v>
+      </c>
+      <c r="R10" s="2">
+        <v>1</v>
+      </c>
+      <c r="S10" s="2">
+        <v>70</v>
+      </c>
+      <c r="T10" s="2">
+        <v>25</v>
+      </c>
+      <c r="U10" s="2">
+        <v>30</v>
+      </c>
+      <c r="V10" s="2">
+        <v>40</v>
+      </c>
+      <c r="W10" s="2">
+        <v>20</v>
+      </c>
+      <c r="X10" s="2">
+        <v>25</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>50</v>
+      </c>
+      <c r="AA10">
+        <f>SUM(S10:Z10)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>106</v>
       </c>
@@ -2443,8 +3116,72 @@
       <c r="F11" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G11" s="2">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>20</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>7</v>
+      </c>
+      <c r="N11">
+        <v>9</v>
+      </c>
+      <c r="O11">
+        <v>5</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>4</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>65</v>
+      </c>
+      <c r="T11">
+        <v>25</v>
+      </c>
+      <c r="U11">
+        <v>5</v>
+      </c>
+      <c r="V11">
+        <v>35</v>
+      </c>
+      <c r="W11">
+        <v>45</v>
+      </c>
+      <c r="X11">
+        <v>20</v>
+      </c>
+      <c r="Y11">
+        <v>5</v>
+      </c>
+      <c r="Z11">
+        <v>40</v>
+      </c>
+      <c r="AA11">
+        <f>SUM(S11:Z11)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -2460,8 +3197,72 @@
       <c r="F12" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G12" s="2">
+        <v>3</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>25</v>
+      </c>
+      <c r="K12">
+        <v>9</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>6</v>
+      </c>
+      <c r="N12">
+        <v>6</v>
+      </c>
+      <c r="O12">
+        <v>8</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="Q12">
+        <v>2</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>80</v>
+      </c>
+      <c r="T12">
+        <v>40</v>
+      </c>
+      <c r="U12">
+        <v>10</v>
+      </c>
+      <c r="V12">
+        <v>30</v>
+      </c>
+      <c r="W12">
+        <v>20</v>
+      </c>
+      <c r="X12">
+        <v>35</v>
+      </c>
+      <c r="Y12">
+        <v>10</v>
+      </c>
+      <c r="Z12">
+        <v>10</v>
+      </c>
+      <c r="AA12">
+        <f>SUM(S12:Z12)</f>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -2474,8 +3275,72 @@
       <c r="F13" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G13" s="2">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>23</v>
+      </c>
+      <c r="K13" s="2">
+        <v>6</v>
+      </c>
+      <c r="L13" s="2">
+        <v>3</v>
+      </c>
+      <c r="M13" s="2">
+        <v>9</v>
+      </c>
+      <c r="N13" s="2">
+        <v>6</v>
+      </c>
+      <c r="O13" s="2">
+        <v>5</v>
+      </c>
+      <c r="P13" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>1</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <v>70</v>
+      </c>
+      <c r="T13" s="2">
+        <v>30</v>
+      </c>
+      <c r="U13" s="2">
+        <v>5</v>
+      </c>
+      <c r="V13" s="2">
+        <v>45</v>
+      </c>
+      <c r="W13" s="2">
+        <v>30</v>
+      </c>
+      <c r="X13" s="2">
+        <v>25</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>30</v>
+      </c>
+      <c r="AA13">
+        <f>SUM(S13:Z13)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -2488,8 +3353,72 @@
       <c r="F14" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G14" s="2">
+        <v>3</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>18</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+      <c r="M14">
+        <v>6</v>
+      </c>
+      <c r="N14">
+        <v>7</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>3</v>
+      </c>
+      <c r="Q14">
+        <v>5</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>50</v>
+      </c>
+      <c r="T14">
+        <v>10</v>
+      </c>
+      <c r="U14">
+        <v>50</v>
+      </c>
+      <c r="V14">
+        <v>40</v>
+      </c>
+      <c r="W14">
+        <v>40</v>
+      </c>
+      <c r="X14">
+        <v>10</v>
+      </c>
+      <c r="Y14">
+        <v>20</v>
+      </c>
+      <c r="Z14">
+        <v>35</v>
+      </c>
+      <c r="AA14">
+        <f>SUM(S14:Z14)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -2505,28 +3434,92 @@
       <c r="F15" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G15" s="2">
+        <v>4</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <v>18</v>
+      </c>
+      <c r="K15">
+        <v>6</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>7</v>
+      </c>
+      <c r="N15">
+        <v>11</v>
+      </c>
+      <c r="O15">
+        <v>5</v>
+      </c>
+      <c r="P15">
+        <v>7</v>
+      </c>
+      <c r="Q15">
+        <v>4</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>65</v>
+      </c>
+      <c r="T15">
+        <v>25</v>
+      </c>
+      <c r="U15">
+        <v>15</v>
+      </c>
+      <c r="V15">
+        <v>35</v>
+      </c>
+      <c r="W15">
+        <v>45</v>
+      </c>
+      <c r="X15">
+        <v>15</v>
+      </c>
+      <c r="Y15">
+        <v>30</v>
+      </c>
+      <c r="Z15">
+        <v>40</v>
+      </c>
+      <c r="AA15">
+        <f>SUM(S15:Z15)</f>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>168</v>
       </c>
@@ -2542,8 +3535,72 @@
       <c r="F20" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>7</v>
+      </c>
+      <c r="H20" t="s">
+        <v>193</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+      <c r="J20">
+        <v>22</v>
+      </c>
+      <c r="K20">
+        <v>6</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>6</v>
+      </c>
+      <c r="N20">
+        <v>7</v>
+      </c>
+      <c r="O20">
+        <v>6</v>
+      </c>
+      <c r="P20">
+        <v>3</v>
+      </c>
+      <c r="Q20">
+        <v>7</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>70</v>
+      </c>
+      <c r="T20">
+        <v>30</v>
+      </c>
+      <c r="U20">
+        <v>10</v>
+      </c>
+      <c r="V20">
+        <v>30</v>
+      </c>
+      <c r="W20">
+        <v>35</v>
+      </c>
+      <c r="X20">
+        <v>25</v>
+      </c>
+      <c r="Y20">
+        <v>20</v>
+      </c>
+      <c r="Z20">
+        <v>40</v>
+      </c>
+      <c r="AA20">
+        <f>SUM(S20:Z20)</f>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>171</v>
       </c>
@@ -2555,6 +3612,95 @@
       </c>
       <c r="F21" t="s">
         <v>133</v>
+      </c>
+      <c r="G21">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>194</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <v>20</v>
+      </c>
+      <c r="K21">
+        <v>7</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>9</v>
+      </c>
+      <c r="N21">
+        <v>6</v>
+      </c>
+      <c r="O21">
+        <v>3</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>7</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>75</v>
+      </c>
+      <c r="T21">
+        <v>35</v>
+      </c>
+      <c r="U21">
+        <v>5</v>
+      </c>
+      <c r="V21">
+        <v>55</v>
+      </c>
+      <c r="W21">
+        <v>40</v>
+      </c>
+      <c r="X21">
+        <v>15</v>
+      </c>
+      <c r="Y21">
+        <v>10</v>
+      </c>
+      <c r="Z21">
+        <v>30</v>
+      </c>
+      <c r="AA21">
+        <f>SUM(S21:Z21)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed character bases to match spreadsheet
To say things are balanced would be a lie. They are not balanced at all. But that can be finetuned later.
</commit_message>
<xml_diff>
--- a/Brainstorming.xlsx
+++ b/Brainstorming.xlsx
@@ -649,7 +649,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-I'd have too many clerics otherwise.</t>
+Yeah, the first act kind of actually needs a cleric after all.</t>
         </r>
       </text>
     </comment>
@@ -2249,8 +2249,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2442,7 +2443,7 @@
         <v>7</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2">
         <v>80</v>
@@ -2798,8 +2799,8 @@
       <c r="E7" t="s">
         <v>120</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>133</v>
+      <c r="F7" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="G7" s="2">
         <v>1</v>

</xml_diff>